<commit_message>
Setup locator type in OR.properties file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSources/LoginTest.xlsx
+++ b/src/main/resources/dataSources/LoginTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="43">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Implemented and Tested Before and After Test through excel.
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSources/LoginTest.xlsx
+++ b/src/main/resources/dataSources/LoginTest.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Login_001" sheetId="1" r:id="rId2"/>
-    <sheet name="Login_002" sheetId="3" r:id="rId3"/>
+    <sheet name="BEFORE_TEST" sheetId="4" r:id="rId2"/>
+    <sheet name="Login_001" sheetId="1" r:id="rId3"/>
+    <sheet name="Login_002" sheetId="3" r:id="rId4"/>
+    <sheet name="AFTER_TEST" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -78,15 +80,6 @@
     <t>L04</t>
   </si>
   <si>
-    <t>L05</t>
-  </si>
-  <si>
-    <t>L06</t>
-  </si>
-  <si>
-    <t>L07</t>
-  </si>
-  <si>
     <t>PageElement</t>
   </si>
   <si>
@@ -141,10 +134,22 @@
     <t>enterText</t>
   </si>
   <si>
+    <t>BEFORE_TEST</t>
+  </si>
+  <si>
+    <t>BT01</t>
+  </si>
+  <si>
+    <t>BT02</t>
+  </si>
+  <si>
+    <t>AFTER_TEST</t>
+  </si>
+  <si>
+    <t>AT01</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -519,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -533,13 +538,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -547,28 +552,24 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -577,10 +578,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="40.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,16 +689,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -623,15 +709,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -642,17 +732,19 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -663,19 +755,17 @@
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -686,96 +776,28 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -798,167 +820,168 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="43.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>